<commit_message>
Updated actions and messages text
[git-p4: depot-paths = "//Abdaw/dev_main/tracks/": change = 465508]
</commit_message>
<xml_diff>
--- a/PRD-n-SRS/List of Tracks messages.xlsx
+++ b/PRD-n-SRS/List of Tracks messages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
   <si>
     <t>CASE</t>
   </si>
@@ -240,6 +240,55 @@
   </si>
   <si>
     <t>Unless clicked Yes or NO</t>
+  </si>
+  <si>
+    <t>Switching to one of Operation Mode while this mode is already active</t>
+  </si>
+  <si>
+    <t>Information</t>
+  </si>
+  <si>
+    <t>Current mode is already active!</t>
+  </si>
+  <si>
+    <t>Unless clicked OK button</t>
+  </si>
+  <si>
+    <t>Will inform user about current mode is already active. No changes will be done.</t>
+  </si>
+  <si>
+    <t>Choosing available Interface from Interface menu</t>
+  </si>
+  <si>
+    <r>
+      <t>Would you like to switch to "</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>interface name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"?</t>
+    </r>
+  </si>
+  <si>
+    <t>Engine will switched to selected mode according to user answer. All Inputs and Outputs will changed too. Tracks will "remember" last state of Operation Mode and recall it by user define.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Engine will switched to selected interface according to user answer. All Inputs and Outputs will changed too. Last preset of State Controlled will be loaded. </t>
   </si>
 </sst>
 </file>
@@ -657,36 +706,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -704,57 +729,84 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -1116,101 +1168,101 @@
   <sheetData>
     <row r="2" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="5"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="25"/>
     </row>
     <row r="4" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="6"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="8"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="28"/>
     </row>
     <row r="5" spans="3:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G28" s="29" t="s">
+      <c r="G28" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="H28" s="30"/>
-      <c r="I28" s="30"/>
-      <c r="J28" s="31"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="34"/>
     </row>
     <row r="29" spans="3:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="9"/>
-      <c r="G29" s="20" t="s">
+      <c r="D29" s="29"/>
+      <c r="G29" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19" t="s">
+      <c r="H29" s="15"/>
+      <c r="I29" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="J29" s="21"/>
+      <c r="J29" s="16"/>
     </row>
     <row r="30" spans="3:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="10">
+      <c r="C30" s="30">
         <v>41791</v>
       </c>
-      <c r="D30" s="10"/>
-      <c r="G30" s="22" t="s">
+      <c r="D30" s="30"/>
+      <c r="G30" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="H30" s="17"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="23"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="18"/>
     </row>
     <row r="31" spans="3:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="G31" s="22"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="24"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="20"/>
     </row>
     <row r="32" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G32" s="25" t="s">
+      <c r="G32" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="H32" s="26"/>
-      <c r="I32" s="27" t="s">
+      <c r="H32" s="13"/>
+      <c r="I32" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="J32" s="28"/>
+      <c r="J32" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:N4"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G28:J28"/>
     <mergeCell ref="G32:H32"/>
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="I29:J29"/>
     <mergeCell ref="I30:J30"/>
     <mergeCell ref="I31:J31"/>
     <mergeCell ref="I32:J32"/>
-    <mergeCell ref="C3:N4"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G28:J28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1219,10 +1271,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G191"/>
+  <dimension ref="A2:G192"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1232,7 +1284,7 @@
   <sheetData>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:7" s="2" customFormat="1" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1255,420 +1307,454 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="34"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="13"/>
+      <c r="A5" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G8" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="33" t="s">
+    <row r="9" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D9" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="15" t="s">
+      <c r="E9" s="5"/>
+      <c r="F9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G9" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="34" t="s">
+    <row r="10" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G10" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="34"/>
-      <c r="B10" s="13" t="s">
+    <row r="11" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="11"/>
+      <c r="B11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D11" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F11" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G11" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="34"/>
-      <c r="B11" s="13" t="s">
+    <row r="12" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="11"/>
+      <c r="B12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D12" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F12" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G12" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="34"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="12"/>
-    </row>
     <row r="13" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="34"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="12"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="34"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="12"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="34"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="12"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="34"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="12"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="34"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="12"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="34"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="12"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="34"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="12"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="34"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="12"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="34"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="12"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="34"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="12"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="34"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="12"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="34"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="12"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="F25" s="32"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="4"/>
+    </row>
+    <row r="25" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="11"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
-      <c r="F26" s="32"/>
+      <c r="F26" s="9"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
-      <c r="F27" s="32"/>
+      <c r="F27" s="9"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
-      <c r="F28" s="32"/>
+      <c r="F28" s="9"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
-      <c r="F29" s="32"/>
+      <c r="F29" s="9"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
-      <c r="F30" s="32"/>
+      <c r="F30" s="9"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
-      <c r="F31" s="32"/>
+      <c r="F31" s="9"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
-      <c r="F32" s="32"/>
+      <c r="F32" s="9"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
-      <c r="F33" s="32"/>
+      <c r="F33" s="9"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
-      <c r="F34" s="32"/>
+      <c r="F34" s="9"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
-      <c r="F35" s="32"/>
+      <c r="F35" s="9"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
-      <c r="F36" s="32"/>
+      <c r="F36" s="9"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
-      <c r="F37" s="32"/>
+      <c r="F37" s="9"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
-      <c r="F38" s="32"/>
+      <c r="F38" s="9"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
-      <c r="F39" s="32"/>
+      <c r="F39" s="9"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
-      <c r="F40" s="32"/>
+      <c r="F40" s="9"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
-      <c r="F41" s="32"/>
+      <c r="F41" s="9"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
-      <c r="F42" s="32"/>
+      <c r="F42" s="9"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
-      <c r="F43" s="32"/>
+      <c r="F43" s="9"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
-      <c r="F44" s="32"/>
+      <c r="F44" s="9"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
-      <c r="F45" s="32"/>
+      <c r="F45" s="9"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
-      <c r="F46" s="32"/>
+      <c r="F46" s="9"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
-      <c r="F47" s="32"/>
+      <c r="F47" s="9"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
-      <c r="F48" s="32"/>
+      <c r="F48" s="9"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
-      <c r="F49" s="32"/>
+      <c r="F49" s="9"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
-      <c r="F50" s="32"/>
+      <c r="F50" s="9"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
-      <c r="F51" s="32"/>
+      <c r="F51" s="9"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
-      <c r="F52" s="32"/>
+      <c r="F52" s="9"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
-      <c r="F53" s="32"/>
+      <c r="F53" s="9"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
-      <c r="F54" s="32"/>
+      <c r="F54" s="9"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
-      <c r="F55" s="32"/>
+      <c r="F55" s="9"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
-      <c r="F56" s="32"/>
+      <c r="F56" s="9"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
-      <c r="F57" s="32"/>
+      <c r="F57" s="9"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
+      <c r="F58" s="9"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
@@ -2068,6 +2154,9 @@
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" s="2"/>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>